<commit_message>
add cyclone_phailin and run topN, shifty on all events
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="59">
   <si>
     <t>Event</t>
   </si>
@@ -64,13 +64,145 @@
   </si>
   <si>
     <t>boston_bombing</t>
+  </si>
+  <si>
+    <t>Iterations</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>2015_03_24_12</t>
+  </si>
+  <si>
+    <t>4U9525</t>
+  </si>
+  <si>
+    <t>charlotte</t>
+  </si>
+  <si>
+    <t>2015_05_02_08</t>
+  </si>
+  <si>
+    <t>chelyabinsk_meteor</t>
+  </si>
+  <si>
+    <t>2013_02_15_07</t>
+  </si>
+  <si>
+    <t>chibok_kidnap</t>
+  </si>
+  <si>
+    <t>2014_04_15_11</t>
+  </si>
+  <si>
+    <t>garissa</t>
+  </si>
+  <si>
+    <t>2015_04_02_06</t>
+  </si>
+  <si>
+    <t>MH17</t>
+  </si>
+  <si>
+    <t>2014_07_17_17</t>
+  </si>
+  <si>
+    <t>nepal_quake</t>
+  </si>
+  <si>
+    <t>2015_04_25_09</t>
+  </si>
+  <si>
+    <t>nepal_quake2</t>
+  </si>
+  <si>
+    <t>2015_05_12_09</t>
+  </si>
+  <si>
+    <t>peshawar_school</t>
+  </si>
+  <si>
+    <t>2014_12_16_09</t>
+  </si>
+  <si>
+    <t>qz8501</t>
+  </si>
+  <si>
+    <t>2014_12_28_05</t>
+  </si>
+  <si>
+    <t>savar_collapse</t>
+  </si>
+  <si>
+    <t>2013_04_24_10</t>
+  </si>
+  <si>
+    <t>typhoon_haiyan</t>
+  </si>
+  <si>
+    <t>2013_11_09_03</t>
+  </si>
+  <si>
+    <t>afghan_landslide</t>
+  </si>
+  <si>
+    <t>2014_05_02_14</t>
+  </si>
+  <si>
+    <t>ontake_eruption</t>
+  </si>
+  <si>
+    <t>2014_09_27_08</t>
+  </si>
+  <si>
+    <t>cyclone_phailin</t>
+  </si>
+  <si>
+    <t>2013_10_11_20</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,13 +221,25 @@
       <name val="Schriftart für Textkörper"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
       <name val="Schriftart für Textkörper"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Schriftart für Textkörper"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Schriftart für Textkörper"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,8 +258,23 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -134,22 +293,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
+    <cellStyle name="Accent4" xfId="5" builtinId="41"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,74 +691,569 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N2"/>
+  <dimension ref="B1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="10.625" style="1"/>
-    <col min="11" max="11" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.625" style="10"/>
+    <col min="2" max="2" width="13.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="10.625" style="10"/>
+    <col min="16" max="16" width="12.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:19" s="1" customFormat="1" ht="16">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:14">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:19">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="G2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+    </row>
+    <row r="3" spans="2:19">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="10">
+        <v>10</v>
+      </c>
+      <c r="E3" s="10">
+        <v>15</v>
+      </c>
+      <c r="G3" s="10">
+        <v>200</v>
+      </c>
+      <c r="H3" s="10">
+        <v>400</v>
+      </c>
+      <c r="I3" s="10">
+        <v>600</v>
+      </c>
+      <c r="J3" s="10">
+        <v>10</v>
+      </c>
+      <c r="K3" s="10">
+        <v>20</v>
+      </c>
+      <c r="L3" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19">
+      <c r="B4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="D5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19">
+      <c r="B6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19">
+      <c r="B7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19">
+      <c r="B8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19">
+      <c r="B9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19">
+      <c r="B10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19">
+      <c r="B11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19">
+      <c r="B12" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19">
+      <c r="B13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19">
+      <c r="B14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19">
+      <c r="B15" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19">
+      <c r="B16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:L2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add docs to scripts and sql
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -697,7 +697,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,12 +739,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1057,7 +1051,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="130">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1083,7 +1077,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1189,7 +1184,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1248,7 +1243,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="4" applyBorder="1"/>
     <xf numFmtId="49" fontId="11" fillId="7" borderId="0" xfId="23" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1269,20 +1264,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="49" fontId="11" fillId="7" borderId="4" xfId="23" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="11" fillId="7" borderId="0" xfId="23" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="25" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1290,8 +1283,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="21" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="21" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1320,11 +1313,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="7" borderId="20" xfId="23" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="130">
+  <cellStyles count="131">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34"/>
-    <cellStyle name="20% - Accent4" xfId="25" builtinId="42"/>
     <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -1335,58 +1328,59 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1397,58 +1391,59 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Neutral" xfId="23" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1784,9 +1779,9 @@
   <dimension ref="A1:BG26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="O26" sqref="O26"/>
+      <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0"/>
@@ -1854,7 +1849,7 @@
       <c r="AD1" s="20"/>
       <c r="AE1" s="20"/>
       <c r="AF1" s="20"/>
-      <c r="AG1" s="67"/>
+      <c r="AG1" s="65"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="20" t="s">
@@ -1913,52 +1908,52 @@
       </c>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
-      <c r="M2" s="78" t="s">
+      <c r="M2" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="N2" s="75"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="80" t="s">
+      <c r="N2" s="73"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="78" t="s">
+      <c r="Q2" s="74"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="T2" s="79"/>
-      <c r="U2" s="80" t="s">
+      <c r="T2" s="77"/>
+      <c r="U2" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="76"/>
-      <c r="W2" s="77"/>
-      <c r="X2" s="78" t="s">
+      <c r="V2" s="74"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="80" t="s">
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="AA2" s="76"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="82" t="s">
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="AD2" s="79"/>
-      <c r="AE2" s="80" t="s">
+      <c r="AD2" s="77"/>
+      <c r="AE2" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="AF2" s="76"/>
-      <c r="AG2" s="81"/>
-      <c r="AH2" s="74" t="s">
+      <c r="AF2" s="74"/>
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="AI2" s="75"/>
-      <c r="AJ2" s="76" t="s">
+      <c r="AI2" s="73"/>
+      <c r="AJ2" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="AK2" s="76"/>
-      <c r="AL2" s="77"/>
+      <c r="AK2" s="74"/>
+      <c r="AL2" s="75"/>
       <c r="AM2" s="55"/>
       <c r="AN2" s="55"/>
       <c r="AO2" s="16" t="s">
@@ -2078,7 +2073,7 @@
       <c r="AF3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AG3" s="68" t="s">
+      <c r="AG3" s="66" t="s">
         <v>61</v>
       </c>
       <c r="AH3" s="56" t="s">
@@ -2209,7 +2204,7 @@
       <c r="AD4" s="57"/>
       <c r="AE4" s="57"/>
       <c r="AF4" s="57"/>
-      <c r="AG4" s="69"/>
+      <c r="AG4" s="67"/>
       <c r="AH4" s="57"/>
       <c r="AI4" s="57"/>
       <c r="AL4" s="61"/>
@@ -2279,7 +2274,7 @@
       <c r="AD5" s="57"/>
       <c r="AE5" s="57"/>
       <c r="AF5" s="57"/>
-      <c r="AG5" s="69"/>
+      <c r="AG5" s="67"/>
       <c r="AH5" s="57"/>
       <c r="AI5" s="57"/>
       <c r="AL5" s="58"/>
@@ -2349,7 +2344,7 @@
       <c r="AD6" s="57"/>
       <c r="AE6" s="57"/>
       <c r="AF6" s="57"/>
-      <c r="AG6" s="69"/>
+      <c r="AG6" s="67"/>
       <c r="AH6" s="57"/>
       <c r="AI6" s="57"/>
       <c r="AL6" s="58"/>
@@ -2419,7 +2414,7 @@
       <c r="AD7" s="57"/>
       <c r="AE7" s="57"/>
       <c r="AF7" s="57"/>
-      <c r="AG7" s="69"/>
+      <c r="AG7" s="67"/>
       <c r="AH7" s="57"/>
       <c r="AI7" s="57"/>
       <c r="AL7" s="58"/>
@@ -2489,7 +2484,7 @@
       <c r="AD8" s="57"/>
       <c r="AE8" s="57"/>
       <c r="AF8" s="57"/>
-      <c r="AG8" s="69"/>
+      <c r="AG8" s="67"/>
       <c r="AH8" s="57"/>
       <c r="AI8" s="57"/>
       <c r="AL8" s="58"/>
@@ -2559,7 +2554,7 @@
       <c r="AD9" s="57"/>
       <c r="AE9" s="57"/>
       <c r="AF9" s="57"/>
-      <c r="AG9" s="69"/>
+      <c r="AG9" s="67"/>
       <c r="AH9" s="57"/>
       <c r="AI9" s="57"/>
       <c r="AL9" s="58"/>
@@ -2629,7 +2624,7 @@
       <c r="AD10" s="57"/>
       <c r="AE10" s="57"/>
       <c r="AF10" s="57"/>
-      <c r="AG10" s="69"/>
+      <c r="AG10" s="67"/>
       <c r="AH10" s="57"/>
       <c r="AI10" s="57"/>
       <c r="AL10" s="58"/>
@@ -2699,7 +2694,7 @@
       <c r="AD11" s="57"/>
       <c r="AE11" s="57"/>
       <c r="AF11" s="57"/>
-      <c r="AG11" s="69"/>
+      <c r="AG11" s="67"/>
       <c r="AH11" s="57"/>
       <c r="AI11" s="57"/>
       <c r="AL11" s="58"/>
@@ -2769,7 +2764,7 @@
       <c r="AD12" s="57"/>
       <c r="AE12" s="57"/>
       <c r="AF12" s="57"/>
-      <c r="AG12" s="69"/>
+      <c r="AG12" s="67"/>
       <c r="AH12" s="57"/>
       <c r="AI12" s="57"/>
       <c r="AL12" s="58"/>
@@ -2839,7 +2834,7 @@
       <c r="AD13" s="57"/>
       <c r="AE13" s="57"/>
       <c r="AF13" s="57"/>
-      <c r="AG13" s="69"/>
+      <c r="AG13" s="67"/>
       <c r="AH13" s="57"/>
       <c r="AI13" s="57"/>
       <c r="AL13" s="58"/>
@@ -2909,7 +2904,7 @@
       <c r="AD14" s="57"/>
       <c r="AE14" s="57"/>
       <c r="AF14" s="57"/>
-      <c r="AG14" s="69"/>
+      <c r="AG14" s="67"/>
       <c r="AH14" s="57"/>
       <c r="AI14" s="57"/>
       <c r="AL14" s="58"/>
@@ -2979,7 +2974,7 @@
       <c r="AD15" s="57"/>
       <c r="AE15" s="57"/>
       <c r="AF15" s="57"/>
-      <c r="AG15" s="69"/>
+      <c r="AG15" s="67"/>
       <c r="AH15" s="57"/>
       <c r="AI15" s="57"/>
       <c r="AL15" s="58"/>
@@ -3049,7 +3044,7 @@
       <c r="AD16" s="57"/>
       <c r="AE16" s="57"/>
       <c r="AF16" s="57"/>
-      <c r="AG16" s="69"/>
+      <c r="AG16" s="67"/>
       <c r="AH16" s="57"/>
       <c r="AI16" s="57"/>
       <c r="AL16" s="58"/>
@@ -3162,7 +3157,7 @@
       <c r="AF17" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AG17" s="70" t="s">
+      <c r="AG17" s="68" t="s">
         <v>47</v>
       </c>
       <c r="AH17" s="34" t="s">
@@ -3325,7 +3320,7 @@
       <c r="AF18" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AG18" s="70" t="s">
+      <c r="AG18" s="68" t="s">
         <v>47</v>
       </c>
       <c r="AH18" s="34" t="s">
@@ -3358,7 +3353,7 @@
       <c r="AQ18" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AR18" s="73" t="s">
+      <c r="AR18" s="71" t="s">
         <v>47</v>
       </c>
       <c r="AS18" s="53" t="s">
@@ -3488,7 +3483,7 @@
       <c r="AF19" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AG19" s="70" t="s">
+      <c r="AG19" s="68" t="s">
         <v>47</v>
       </c>
       <c r="AH19" s="34" t="s">
@@ -3506,7 +3501,7 @@
       <c r="AL19" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AM19" s="73" t="s">
+      <c r="AM19" s="71" t="s">
         <v>47</v>
       </c>
       <c r="AN19" s="53" t="s">
@@ -3521,7 +3516,7 @@
       <c r="AQ19" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AR19" s="73" t="s">
+      <c r="AR19" s="71" t="s">
         <v>47</v>
       </c>
       <c r="AS19" s="53" t="s">
@@ -3651,7 +3646,7 @@
       <c r="AF20" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AG20" s="70" t="s">
+      <c r="AG20" s="68" t="s">
         <v>47</v>
       </c>
       <c r="AH20" s="34" t="s">
@@ -3684,7 +3679,7 @@
       <c r="AQ20" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AR20" s="73" t="s">
+      <c r="AR20" s="71" t="s">
         <v>47</v>
       </c>
       <c r="AS20" s="53" t="s">
@@ -3814,7 +3809,7 @@
       <c r="AF21" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AG21" s="70" t="s">
+      <c r="AG21" s="68" t="s">
         <v>47</v>
       </c>
       <c r="AH21" s="34" t="s">
@@ -3845,7 +3840,7 @@
       <c r="AQ21" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AR21" s="73" t="s">
+      <c r="AR21" s="71" t="s">
         <v>47</v>
       </c>
       <c r="AS21" s="53" t="s">
@@ -3975,7 +3970,7 @@
       <c r="AF22" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="AG22" s="71" t="s">
+      <c r="AG22" s="69" t="s">
         <v>50</v>
       </c>
       <c r="AH22" s="34" t="s">
@@ -4006,7 +4001,7 @@
       <c r="AQ22" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AR22" s="73" t="s">
+      <c r="AR22" s="71" t="s">
         <v>47</v>
       </c>
       <c r="AS22" s="53" t="s">
@@ -4136,7 +4131,7 @@
       <c r="AF23" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="AG23" s="72" t="s">
+      <c r="AG23" s="70" t="s">
         <v>47</v>
       </c>
       <c r="AH23" s="34" t="s">
@@ -4167,7 +4162,7 @@
       <c r="AQ23" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AR23" s="73"/>
+      <c r="AR23" s="71"/>
       <c r="AS23" s="53"/>
       <c r="AT23" s="53" t="s">
         <v>47</v>
@@ -4293,7 +4288,7 @@
       <c r="AF24" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="AG24" s="72" t="s">
+      <c r="AG24" s="70" t="s">
         <v>47</v>
       </c>
       <c r="AH24" s="54" t="s">
@@ -4311,7 +4306,7 @@
       <c r="AL24" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AM24" s="83" t="s">
+      <c r="AM24" s="81" t="s">
         <v>104</v>
       </c>
       <c r="AN24" s="54" t="s">
@@ -4452,7 +4447,7 @@
       <c r="AF25" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="AG25" s="72" t="s">
+      <c r="AG25" s="70" t="s">
         <v>47</v>
       </c>
       <c r="AH25" s="34" t="s">
@@ -4522,13 +4517,13 @@
       <c r="BD25"/>
     </row>
     <row r="26" spans="1:56">
-      <c r="B26" s="65" t="s">
+      <c r="B26" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="34" t="s">
         <v>66</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -4615,7 +4610,7 @@
       <c r="AF26" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="AG26" s="72" t="s">
+      <c r="AG26" s="70" t="s">
         <v>47</v>
       </c>
       <c r="AH26" s="34" t="s">

</xml_diff>